<commit_message>
Atualização da base de dados
</commit_message>
<xml_diff>
--- a/dados/2025-1_GestaoResultado_ResumoInscricoes_GRAD.xlsx
+++ b/dados/2025-1_GestaoResultado_ResumoInscricoes_GRAD.xlsx
@@ -824,7 +824,7 @@
         <x:v>11</x:v>
       </x:c>
       <x:c r="E4" s="0" t="n">
-        <x:v>3</x:v>
+        <x:v>5</x:v>
       </x:c>
       <x:c r="F4" s="0" t="n">
         <x:v>0</x:v>
@@ -1110,16 +1110,16 @@
         <x:v>11</x:v>
       </x:c>
       <x:c r="E15" s="0" t="n">
-        <x:v>81</x:v>
+        <x:v>86</x:v>
       </x:c>
       <x:c r="F15" s="0" t="n">
-        <x:v>36</x:v>
+        <x:v>37</x:v>
       </x:c>
       <x:c r="G15" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H15" s="0" t="n">
-        <x:v>36</x:v>
+        <x:v>37</x:v>
       </x:c>
     </x:row>
     <x:row r="16" spans="1:8">
@@ -1162,7 +1162,7 @@
         <x:v>11</x:v>
       </x:c>
       <x:c r="E17" s="0" t="n">
-        <x:v>48</x:v>
+        <x:v>51</x:v>
       </x:c>
       <x:c r="F17" s="0" t="n">
         <x:v>17</x:v>
@@ -1188,7 +1188,7 @@
         <x:v>11</x:v>
       </x:c>
       <x:c r="E18" s="0" t="n">
-        <x:v>45</x:v>
+        <x:v>46</x:v>
       </x:c>
       <x:c r="F18" s="0" t="n">
         <x:v>11</x:v>
@@ -1214,7 +1214,7 @@
         <x:v>11</x:v>
       </x:c>
       <x:c r="E19" s="0" t="n">
-        <x:v>23</x:v>
+        <x:v>24</x:v>
       </x:c>
       <x:c r="F19" s="0" t="n">
         <x:v>16</x:v>
@@ -1578,7 +1578,7 @@
         <x:v>11</x:v>
       </x:c>
       <x:c r="E33" s="0" t="n">
-        <x:v>14</x:v>
+        <x:v>15</x:v>
       </x:c>
       <x:c r="F33" s="0" t="n">
         <x:v>6</x:v>
@@ -1786,16 +1786,16 @@
         <x:v>11</x:v>
       </x:c>
       <x:c r="E41" s="0" t="n">
-        <x:v>14</x:v>
+        <x:v>15</x:v>
       </x:c>
       <x:c r="F41" s="0" t="n">
-        <x:v>5</x:v>
+        <x:v>6</x:v>
       </x:c>
       <x:c r="G41" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H41" s="0" t="n">
-        <x:v>5</x:v>
+        <x:v>6</x:v>
       </x:c>
     </x:row>
     <x:row r="42" spans="1:8">
@@ -1916,16 +1916,16 @@
         <x:v>11</x:v>
       </x:c>
       <x:c r="E46" s="0" t="n">
-        <x:v>11</x:v>
+        <x:v>13</x:v>
       </x:c>
       <x:c r="F46" s="0" t="n">
-        <x:v>0</x:v>
+        <x:v>1</x:v>
       </x:c>
       <x:c r="G46" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H46" s="0" t="n">
-        <x:v>0</x:v>
+        <x:v>1</x:v>
       </x:c>
     </x:row>
     <x:row r="47" spans="1:8">
@@ -1968,16 +1968,16 @@
         <x:v>11</x:v>
       </x:c>
       <x:c r="E48" s="0" t="n">
-        <x:v>7</x:v>
+        <x:v>9</x:v>
       </x:c>
       <x:c r="F48" s="0" t="n">
-        <x:v>3</x:v>
+        <x:v>5</x:v>
       </x:c>
       <x:c r="G48" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H48" s="0" t="n">
-        <x:v>3</x:v>
+        <x:v>5</x:v>
       </x:c>
     </x:row>
     <x:row r="49" spans="1:8">
@@ -1994,16 +1994,16 @@
         <x:v>11</x:v>
       </x:c>
       <x:c r="E49" s="0" t="n">
-        <x:v>24</x:v>
+        <x:v>25</x:v>
       </x:c>
       <x:c r="F49" s="0" t="n">
-        <x:v>11</x:v>
+        <x:v>12</x:v>
       </x:c>
       <x:c r="G49" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H49" s="0" t="n">
-        <x:v>11</x:v>
+        <x:v>12</x:v>
       </x:c>
     </x:row>
     <x:row r="50" spans="1:8">
@@ -2384,16 +2384,16 @@
         <x:v>11</x:v>
       </x:c>
       <x:c r="E64" s="0" t="n">
-        <x:v>19</x:v>
+        <x:v>20</x:v>
       </x:c>
       <x:c r="F64" s="0" t="n">
-        <x:v>9</x:v>
+        <x:v>10</x:v>
       </x:c>
       <x:c r="G64" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H64" s="0" t="n">
-        <x:v>9</x:v>
+        <x:v>10</x:v>
       </x:c>
     </x:row>
     <x:row r="65" spans="1:8">
@@ -2410,7 +2410,7 @@
         <x:v>11</x:v>
       </x:c>
       <x:c r="E65" s="0" t="n">
-        <x:v>12</x:v>
+        <x:v>14</x:v>
       </x:c>
       <x:c r="F65" s="0" t="n">
         <x:v>4</x:v>
@@ -2436,7 +2436,7 @@
         <x:v>11</x:v>
       </x:c>
       <x:c r="E66" s="0" t="n">
-        <x:v>17</x:v>
+        <x:v>18</x:v>
       </x:c>
       <x:c r="F66" s="0" t="n">
         <x:v>8</x:v>
@@ -2566,7 +2566,7 @@
         <x:v>11</x:v>
       </x:c>
       <x:c r="E71" s="0" t="n">
-        <x:v>8</x:v>
+        <x:v>9</x:v>
       </x:c>
       <x:c r="F71" s="0" t="n">
         <x:v>5</x:v>
@@ -2774,7 +2774,7 @@
         <x:v>11</x:v>
       </x:c>
       <x:c r="E79" s="0" t="n">
-        <x:v>5</x:v>
+        <x:v>10</x:v>
       </x:c>
       <x:c r="F79" s="0" t="n">
         <x:v>3</x:v>
@@ -2800,7 +2800,7 @@
         <x:v>11</x:v>
       </x:c>
       <x:c r="E80" s="0" t="n">
-        <x:v>12</x:v>
+        <x:v>15</x:v>
       </x:c>
       <x:c r="F80" s="0" t="n">
         <x:v>5</x:v>

</xml_diff>